<commit_message>
A whole bunch of stuff again
Add test of differences
</commit_message>
<xml_diff>
--- a/data/Data_fish_YC.xlsx
+++ b/data/Data_fish_YC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgilbe01\Desktop\PhD_2020-2023_09\01.Analyses\Ker_Arctgazella-prey-poop\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F79FE18-625C-42EC-9705-B68B86552D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FABEEC-9EA5-4496-A954-05A4F08DADDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31470" yWindow="2250" windowWidth="19425" windowHeight="10425" tabRatio="1000" xr2:uid="{63FB60A9-7299-4E64-8198-9CD82964FF61}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" xr2:uid="{63FB60A9-7299-4E64-8198-9CD82964FF61}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2384,9 +2384,6 @@
     <t>2010PII_MANCMAN_MM1_st66_C</t>
   </si>
   <si>
-    <t>Notolepsis coatsi</t>
-  </si>
-  <si>
     <t>2005_NOTOCOA_NC01</t>
   </si>
   <si>
@@ -2520,6 +2517,9 @@
   </si>
   <si>
     <t>Melamphaidae</t>
+  </si>
+  <si>
+    <t>Notolepis coatsi</t>
   </si>
 </sst>
 </file>
@@ -8783,7 +8783,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AB5AB86-2C13-4A63-BEBB-F18724BA41E0}" name="Tableau croisé dynamique2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AB5AB86-2C13-4A63-BEBB-F18724BA41E0}" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="21">
     <pivotField showAll="0">
@@ -10030,7 +10030,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -10329,14 +10329,14 @@
   <dimension ref="A1:V511"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="12000" ySplit="705" topLeftCell="N403" activePane="bottomLeft"/>
+      <pane xSplit="12000" ySplit="705" topLeftCell="N472" activePane="bottomLeft"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="G3" sqref="G1:G1048576"/>
-      <selection pane="bottomLeft" activeCell="A413" sqref="A413"/>
+      <selection pane="bottomLeft" activeCell="B480" sqref="B480"/>
       <selection pane="bottomRight" activeCell="S163" sqref="S163:S164"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.26953125" bestFit="1" customWidth="1"/>
@@ -10427,7 +10427,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -10493,7 +10493,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -10559,7 +10559,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
@@ -10625,7 +10625,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -10691,7 +10691,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
@@ -10757,7 +10757,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
@@ -10823,7 +10823,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -10889,7 +10889,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
@@ -10955,7 +10955,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -11021,7 +11021,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
@@ -11087,7 +11087,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
@@ -11153,7 +11153,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
@@ -11216,7 +11216,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B14" t="s">
         <v>45</v>
@@ -11282,7 +11282,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B15" t="s">
         <v>45</v>
@@ -11348,7 +11348,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
@@ -11414,7 +11414,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B17" t="s">
         <v>45</v>
@@ -11480,7 +11480,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B18" t="s">
         <v>45</v>
@@ -11546,7 +11546,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B19" t="s">
         <v>45</v>
@@ -11612,7 +11612,7 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B20" t="s">
         <v>45</v>
@@ -11678,7 +11678,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B21" t="s">
         <v>45</v>
@@ -11744,7 +11744,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B22" t="s">
         <v>45</v>
@@ -11810,7 +11810,7 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B23" t="s">
         <v>45</v>
@@ -11876,7 +11876,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B24" t="s">
         <v>45</v>
@@ -11942,7 +11942,7 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B25" t="s">
         <v>45</v>
@@ -12008,7 +12008,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B26" t="s">
         <v>45</v>
@@ -12074,7 +12074,7 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B27" t="s">
         <v>45</v>
@@ -12137,7 +12137,7 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B28" t="s">
         <v>137</v>
@@ -12203,7 +12203,7 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B29" t="s">
         <v>137</v>
@@ -12269,7 +12269,7 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B30" t="s">
         <v>137</v>
@@ -12335,7 +12335,7 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B31" t="s">
         <v>137</v>
@@ -12401,7 +12401,7 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B32" t="s">
         <v>137</v>
@@ -12467,7 +12467,7 @@
     </row>
     <row r="33" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>137</v>
@@ -12536,7 +12536,7 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B34" t="s">
         <v>137</v>
@@ -12602,7 +12602,7 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B35" t="s">
         <v>137</v>
@@ -12668,7 +12668,7 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B36" t="s">
         <v>137</v>
@@ -12734,7 +12734,7 @@
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B37" t="s">
         <v>137</v>
@@ -12800,7 +12800,7 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B38" t="s">
         <v>137</v>
@@ -12866,7 +12866,7 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B39" t="s">
         <v>137</v>
@@ -12932,7 +12932,7 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B40" t="s">
         <v>28</v>
@@ -12998,7 +12998,7 @@
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B41" t="s">
         <v>28</v>
@@ -13064,7 +13064,7 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B42" t="s">
         <v>28</v>
@@ -13130,7 +13130,7 @@
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B43" t="s">
         <v>28</v>
@@ -13196,7 +13196,7 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B44" t="s">
         <v>28</v>
@@ -13262,7 +13262,7 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B45" t="s">
         <v>28</v>
@@ -13328,7 +13328,7 @@
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B46" t="s">
         <v>28</v>
@@ -13394,7 +13394,7 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B47" t="s">
         <v>28</v>
@@ -13460,7 +13460,7 @@
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B48" t="s">
         <v>28</v>
@@ -13526,7 +13526,7 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B49" t="s">
         <v>28</v>
@@ -13592,7 +13592,7 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B50" t="s">
         <v>28</v>
@@ -13658,7 +13658,7 @@
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B51" t="s">
         <v>28</v>
@@ -13724,7 +13724,7 @@
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B52" t="s">
         <v>62</v>
@@ -13790,7 +13790,7 @@
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B53" t="s">
         <v>62</v>
@@ -13856,7 +13856,7 @@
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B54" t="s">
         <v>62</v>
@@ -13922,7 +13922,7 @@
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B55" t="s">
         <v>62</v>
@@ -13988,7 +13988,7 @@
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B56" t="s">
         <v>40</v>
@@ -14054,7 +14054,7 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B57" t="s">
         <v>40</v>
@@ -14120,7 +14120,7 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B58" t="s">
         <v>40</v>
@@ -14186,7 +14186,7 @@
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B59" t="s">
         <v>40</v>
@@ -14252,7 +14252,7 @@
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B60" t="s">
         <v>31</v>
@@ -14318,7 +14318,7 @@
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B61" t="s">
         <v>31</v>
@@ -14384,7 +14384,7 @@
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B62" t="s">
         <v>31</v>
@@ -14450,7 +14450,7 @@
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B63" t="s">
         <v>31</v>
@@ -14516,7 +14516,7 @@
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B64" t="s">
         <v>29</v>
@@ -14582,7 +14582,7 @@
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B65" t="s">
         <v>29</v>
@@ -14648,7 +14648,7 @@
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B66" t="s">
         <v>29</v>
@@ -14714,7 +14714,7 @@
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B67" t="s">
         <v>29</v>
@@ -14780,7 +14780,7 @@
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B68" t="s">
         <v>29</v>
@@ -14846,7 +14846,7 @@
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B69" t="s">
         <v>29</v>
@@ -14912,7 +14912,7 @@
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B70" t="s">
         <v>29</v>
@@ -14978,7 +14978,7 @@
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B71" t="s">
         <v>29</v>
@@ -15044,7 +15044,7 @@
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B72" t="s">
         <v>55</v>
@@ -15110,7 +15110,7 @@
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B73" t="s">
         <v>55</v>
@@ -15176,7 +15176,7 @@
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B74" t="s">
         <v>55</v>
@@ -15242,7 +15242,7 @@
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B75" t="s">
         <v>55</v>
@@ -15308,7 +15308,7 @@
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B76" t="s">
         <v>55</v>
@@ -15374,7 +15374,7 @@
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B77" t="s">
         <v>55</v>
@@ -15440,7 +15440,7 @@
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B78" t="s">
         <v>55</v>
@@ -15506,7 +15506,7 @@
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B79" t="s">
         <v>55</v>
@@ -15572,7 +15572,7 @@
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B80" t="s">
         <v>55</v>
@@ -15638,7 +15638,7 @@
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B81" t="s">
         <v>55</v>
@@ -15704,7 +15704,7 @@
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B82" t="s">
         <v>55</v>
@@ -15770,7 +15770,7 @@
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B83" t="s">
         <v>135</v>
@@ -15836,7 +15836,7 @@
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B84" t="s">
         <v>135</v>
@@ -15902,7 +15902,7 @@
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B85" t="s">
         <v>135</v>
@@ -15968,7 +15968,7 @@
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B86" t="s">
         <v>135</v>
@@ -16034,7 +16034,7 @@
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B87" t="s">
         <v>135</v>
@@ -16100,7 +16100,7 @@
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B88" t="s">
         <v>135</v>
@@ -16166,7 +16166,7 @@
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B89" t="s">
         <v>135</v>
@@ -16232,7 +16232,7 @@
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B90" t="s">
         <v>135</v>
@@ -16298,7 +16298,7 @@
     </row>
     <row r="91" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B91" t="s">
         <v>135</v>
@@ -16364,7 +16364,7 @@
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B92" t="s">
         <v>135</v>
@@ -16430,7 +16430,7 @@
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B93" t="s">
         <v>135</v>
@@ -16496,7 +16496,7 @@
     </row>
     <row r="94" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B94" t="s">
         <v>153</v>
@@ -16562,7 +16562,7 @@
     </row>
     <row r="95" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B95" t="s">
         <v>153</v>
@@ -16628,7 +16628,7 @@
     </row>
     <row r="96" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B96" t="s">
         <v>153</v>
@@ -16697,7 +16697,7 @@
     </row>
     <row r="97" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B97" t="s">
         <v>153</v>
@@ -16763,7 +16763,7 @@
     </row>
     <row r="98" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B98" t="s">
         <v>153</v>
@@ -16829,7 +16829,7 @@
     </row>
     <row r="99" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B99" t="s">
         <v>153</v>
@@ -16898,7 +16898,7 @@
     </row>
     <row r="100" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B100" t="s">
         <v>153</v>
@@ -16964,7 +16964,7 @@
     </row>
     <row r="101" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B101" t="s">
         <v>153</v>
@@ -17030,7 +17030,7 @@
     </row>
     <row r="102" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B102" t="s">
         <v>153</v>
@@ -17099,7 +17099,7 @@
     </row>
     <row r="103" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B103" t="s">
         <v>153</v>
@@ -17165,7 +17165,7 @@
     </row>
     <row r="104" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B104" t="s">
         <v>153</v>
@@ -17231,7 +17231,7 @@
     </row>
     <row r="105" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B105" t="s">
         <v>153</v>
@@ -17300,7 +17300,7 @@
     </row>
     <row r="106" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B106" s="11" t="s">
         <v>153</v>
@@ -17366,7 +17366,7 @@
     </row>
     <row r="107" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B107" t="s">
         <v>153</v>
@@ -17432,7 +17432,7 @@
     </row>
     <row r="108" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B108" t="s">
         <v>153</v>
@@ -17501,7 +17501,7 @@
     </row>
     <row r="109" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B109" t="s">
         <v>153</v>
@@ -17567,7 +17567,7 @@
     </row>
     <row r="110" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B110" t="s">
         <v>153</v>
@@ -17633,7 +17633,7 @@
     </row>
     <row r="111" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B111" t="s">
         <v>153</v>
@@ -17700,7 +17700,7 @@
     </row>
     <row r="112" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B112" s="9" t="s">
         <v>153</v>
@@ -17769,7 +17769,7 @@
     </row>
     <row r="113" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B113" t="s">
         <v>153</v>
@@ -17835,7 +17835,7 @@
     </row>
     <row r="114" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B114" t="s">
         <v>153</v>
@@ -17902,7 +17902,7 @@
     </row>
     <row r="115" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B115" t="s">
         <v>153</v>
@@ -17968,7 +17968,7 @@
     </row>
     <row r="116" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B116" t="s">
         <v>153</v>
@@ -18034,7 +18034,7 @@
     </row>
     <row r="117" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B117" t="s">
         <v>153</v>
@@ -18101,7 +18101,7 @@
     </row>
     <row r="118" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B118" t="s">
         <v>153</v>
@@ -18167,7 +18167,7 @@
     </row>
     <row r="119" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B119" t="s">
         <v>153</v>
@@ -18233,7 +18233,7 @@
     </row>
     <row r="120" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B120" t="s">
         <v>153</v>
@@ -18302,7 +18302,7 @@
     </row>
     <row r="121" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B121" t="s">
         <v>153</v>
@@ -18368,7 +18368,7 @@
     </row>
     <row r="122" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B122" t="s">
         <v>153</v>
@@ -18434,7 +18434,7 @@
     </row>
     <row r="123" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B123" t="s">
         <v>153</v>
@@ -18503,7 +18503,7 @@
     </row>
     <row r="124" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B124" t="s">
         <v>153</v>
@@ -18569,7 +18569,7 @@
     </row>
     <row r="125" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>153</v>
@@ -18638,7 +18638,7 @@
     </row>
     <row r="126" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B126" s="11" t="s">
         <v>153</v>
@@ -18707,7 +18707,7 @@
     </row>
     <row r="127" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B127" t="s">
         <v>153</v>
@@ -18773,7 +18773,7 @@
     </row>
     <row r="128" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B128" t="s">
         <v>153</v>
@@ -18839,7 +18839,7 @@
     </row>
     <row r="129" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B129" t="s">
         <v>153</v>
@@ -18906,7 +18906,7 @@
     </row>
     <row r="130" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B130" t="s">
         <v>62</v>
@@ -18972,7 +18972,7 @@
     </row>
     <row r="131" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B131" t="s">
         <v>62</v>
@@ -19038,7 +19038,7 @@
     </row>
     <row r="132" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B132" t="s">
         <v>62</v>
@@ -19104,7 +19104,7 @@
     </row>
     <row r="133" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B133" t="s">
         <v>62</v>
@@ -19170,7 +19170,7 @@
     </row>
     <row r="134" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B134" t="s">
         <v>62</v>
@@ -19236,7 +19236,7 @@
     </row>
     <row r="135" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B135" t="s">
         <v>62</v>
@@ -19302,7 +19302,7 @@
     </row>
     <row r="136" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B136" t="s">
         <v>62</v>
@@ -19368,7 +19368,7 @@
     </row>
     <row r="137" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B137" t="s">
         <v>62</v>
@@ -19434,7 +19434,7 @@
     </row>
     <row r="138" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B138" t="s">
         <v>182</v>
@@ -19500,7 +19500,7 @@
     </row>
     <row r="139" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B139" t="s">
         <v>182</v>
@@ -19566,7 +19566,7 @@
     </row>
     <row r="140" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B140" t="s">
         <v>182</v>
@@ -19632,7 +19632,7 @@
     </row>
     <row r="141" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B141" t="s">
         <v>182</v>
@@ -19698,7 +19698,7 @@
     </row>
     <row r="142" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B142" t="s">
         <v>182</v>
@@ -19764,7 +19764,7 @@
     </row>
     <row r="143" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B143" t="s">
         <v>182</v>
@@ -19830,7 +19830,7 @@
     </row>
     <row r="144" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B144" t="s">
         <v>182</v>
@@ -19896,7 +19896,7 @@
     </row>
     <row r="145" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B145" t="s">
         <v>182</v>
@@ -19962,7 +19962,7 @@
     </row>
     <row r="146" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B146" t="s">
         <v>182</v>
@@ -20028,7 +20028,7 @@
     </row>
     <row r="147" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B147" t="s">
         <v>182</v>
@@ -20094,7 +20094,7 @@
     </row>
     <row r="148" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B148" t="s">
         <v>182</v>
@@ -20160,7 +20160,7 @@
     </row>
     <row r="149" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B149" t="s">
         <v>182</v>
@@ -20226,7 +20226,7 @@
     </row>
     <row r="150" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B150" t="s">
         <v>153</v>
@@ -20292,7 +20292,7 @@
     </row>
     <row r="151" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B151" t="s">
         <v>153</v>
@@ -20358,7 +20358,7 @@
     </row>
     <row r="152" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B152" t="s">
         <v>153</v>
@@ -20415,7 +20415,7 @@
     </row>
     <row r="153" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B153" t="s">
         <v>153</v>
@@ -20478,7 +20478,7 @@
     </row>
     <row r="154" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B154" t="s">
         <v>153</v>
@@ -20541,7 +20541,7 @@
     </row>
     <row r="155" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B155" t="s">
         <v>153</v>
@@ -20604,7 +20604,7 @@
     </row>
     <row r="156" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B156" t="s">
         <v>153</v>
@@ -20667,7 +20667,7 @@
     </row>
     <row r="157" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B157" t="s">
         <v>153</v>
@@ -20730,7 +20730,7 @@
     </row>
     <row r="158" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B158" t="s">
         <v>153</v>
@@ -20787,7 +20787,7 @@
     </row>
     <row r="159" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B159" t="s">
         <v>153</v>
@@ -20850,7 +20850,7 @@
     </row>
     <row r="160" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B160" t="s">
         <v>153</v>
@@ -20913,7 +20913,7 @@
     </row>
     <row r="161" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B161" t="s">
         <v>153</v>
@@ -20970,7 +20970,7 @@
     </row>
     <row r="162" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B162" t="s">
         <v>153</v>
@@ -21036,7 +21036,7 @@
     </row>
     <row r="163" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B163" t="s">
         <v>153</v>
@@ -21102,7 +21102,7 @@
     </row>
     <row r="164" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B164" t="s">
         <v>153</v>
@@ -21159,7 +21159,7 @@
     </row>
     <row r="165" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B165" t="s">
         <v>62</v>
@@ -21225,7 +21225,7 @@
     </row>
     <row r="166" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>62</v>
@@ -21295,7 +21295,7 @@
     </row>
     <row r="167" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B167" t="s">
         <v>62</v>
@@ -21361,7 +21361,7 @@
     </row>
     <row r="168" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B168" t="s">
         <v>62</v>
@@ -21427,7 +21427,7 @@
     </row>
     <row r="169" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B169" t="s">
         <v>62</v>
@@ -21493,7 +21493,7 @@
     </row>
     <row r="170" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B170" t="s">
         <v>62</v>
@@ -21559,7 +21559,7 @@
     </row>
     <row r="171" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B171" t="s">
         <v>62</v>
@@ -21625,7 +21625,7 @@
     </row>
     <row r="172" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B172" t="s">
         <v>62</v>
@@ -21691,7 +21691,7 @@
     </row>
     <row r="173" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B173" t="s">
         <v>62</v>
@@ -21757,7 +21757,7 @@
     </row>
     <row r="174" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B174" t="s">
         <v>62</v>
@@ -21823,7 +21823,7 @@
     </row>
     <row r="175" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B175" t="s">
         <v>62</v>
@@ -21889,7 +21889,7 @@
     </row>
     <row r="176" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B176" t="s">
         <v>62</v>
@@ -21955,7 +21955,7 @@
     </row>
     <row r="177" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B177" t="s">
         <v>62</v>
@@ -22021,7 +22021,7 @@
     </row>
     <row r="178" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B178" t="s">
         <v>62</v>
@@ -22087,7 +22087,7 @@
     </row>
     <row r="179" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B179" t="s">
         <v>62</v>
@@ -22153,7 +22153,7 @@
     </row>
     <row r="180" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B180" t="s">
         <v>62</v>
@@ -22219,7 +22219,7 @@
     </row>
     <row r="181" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B181" t="s">
         <v>62</v>
@@ -22285,7 +22285,7 @@
     </row>
     <row r="182" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B182" t="s">
         <v>62</v>
@@ -22351,7 +22351,7 @@
     </row>
     <row r="183" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B183" t="s">
         <v>62</v>
@@ -22417,7 +22417,7 @@
     </row>
     <row r="184" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B184" t="s">
         <v>62</v>
@@ -22483,7 +22483,7 @@
     </row>
     <row r="185" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B185" t="s">
         <v>62</v>
@@ -22549,7 +22549,7 @@
     </row>
     <row r="186" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B186" t="s">
         <v>62</v>
@@ -22615,7 +22615,7 @@
     </row>
     <row r="187" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B187" t="s">
         <v>182</v>
@@ -22681,7 +22681,7 @@
     </row>
     <row r="188" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B188" t="s">
         <v>182</v>
@@ -22747,7 +22747,7 @@
     </row>
     <row r="189" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B189" t="s">
         <v>182</v>
@@ -22813,7 +22813,7 @@
     </row>
     <row r="190" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B190" t="s">
         <v>182</v>
@@ -22879,7 +22879,7 @@
     </row>
     <row r="191" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B191" t="s">
         <v>182</v>
@@ -22945,7 +22945,7 @@
     </row>
     <row r="192" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B192" s="9" t="s">
         <v>182</v>
@@ -23014,7 +23014,7 @@
     </row>
     <row r="193" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B193" s="9" t="s">
         <v>182</v>
@@ -23083,7 +23083,7 @@
     </row>
     <row r="194" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B194" s="9" t="s">
         <v>182</v>
@@ -23152,7 +23152,7 @@
     </row>
     <row r="195" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B195" s="9" t="s">
         <v>182</v>
@@ -23221,7 +23221,7 @@
     </row>
     <row r="196" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B196" t="s">
         <v>182</v>
@@ -23287,7 +23287,7 @@
     </row>
     <row r="197" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B197" t="s">
         <v>182</v>
@@ -23353,7 +23353,7 @@
     </row>
     <row r="198" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B198" t="s">
         <v>182</v>
@@ -23419,7 +23419,7 @@
     </row>
     <row r="199" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B199" t="s">
         <v>182</v>
@@ -23485,7 +23485,7 @@
     </row>
     <row r="200" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B200" t="s">
         <v>182</v>
@@ -23551,7 +23551,7 @@
     </row>
     <row r="201" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B201" t="s">
         <v>182</v>
@@ -23617,7 +23617,7 @@
     </row>
     <row r="202" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B202" t="s">
         <v>182</v>
@@ -23683,7 +23683,7 @@
     </row>
     <row r="203" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B203" t="s">
         <v>264</v>
@@ -23749,7 +23749,7 @@
     </row>
     <row r="204" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B204" t="s">
         <v>264</v>
@@ -23815,7 +23815,7 @@
     </row>
     <row r="205" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B205" t="s">
         <v>264</v>
@@ -23881,7 +23881,7 @@
     </row>
     <row r="206" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B206" t="s">
         <v>264</v>
@@ -23947,7 +23947,7 @@
     </row>
     <row r="207" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B207" t="s">
         <v>264</v>
@@ -24013,7 +24013,7 @@
     </row>
     <row r="208" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B208" t="s">
         <v>264</v>
@@ -24079,7 +24079,7 @@
     </row>
     <row r="209" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B209" t="s">
         <v>264</v>
@@ -24145,7 +24145,7 @@
     </row>
     <row r="210" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B210" t="s">
         <v>264</v>
@@ -24211,7 +24211,7 @@
     </row>
     <row r="211" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B211" t="s">
         <v>264</v>
@@ -24277,7 +24277,7 @@
     </row>
     <row r="212" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B212" t="s">
         <v>264</v>
@@ -24343,7 +24343,7 @@
     </row>
     <row r="213" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B213" t="s">
         <v>264</v>
@@ -24409,7 +24409,7 @@
     </row>
     <row r="214" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B214" t="s">
         <v>62</v>
@@ -24475,7 +24475,7 @@
     </row>
     <row r="215" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B215" t="s">
         <v>62</v>
@@ -24541,7 +24541,7 @@
     </row>
     <row r="216" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B216" t="s">
         <v>62</v>
@@ -24607,7 +24607,7 @@
     </row>
     <row r="217" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B217" t="s">
         <v>62</v>
@@ -24673,7 +24673,7 @@
     </row>
     <row r="218" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B218" t="s">
         <v>62</v>
@@ -24739,7 +24739,7 @@
     </row>
     <row r="219" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B219" t="s">
         <v>62</v>
@@ -24805,7 +24805,7 @@
     </row>
     <row r="220" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B220" t="s">
         <v>62</v>
@@ -24871,7 +24871,7 @@
     </row>
     <row r="221" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B221" t="s">
         <v>62</v>
@@ -24937,7 +24937,7 @@
     </row>
     <row r="222" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B222" t="s">
         <v>62</v>
@@ -25003,7 +25003,7 @@
     </row>
     <row r="223" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B223" t="s">
         <v>62</v>
@@ -25069,7 +25069,7 @@
     </row>
     <row r="224" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B224" t="s">
         <v>62</v>
@@ -25135,7 +25135,7 @@
     </row>
     <row r="225" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B225" t="s">
         <v>62</v>
@@ -25201,7 +25201,7 @@
     </row>
     <row r="226" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B226" t="s">
         <v>264</v>
@@ -25267,7 +25267,7 @@
     </row>
     <row r="227" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B227" t="s">
         <v>264</v>
@@ -25333,7 +25333,7 @@
     </row>
     <row r="228" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B228" t="s">
         <v>264</v>
@@ -25399,7 +25399,7 @@
     </row>
     <row r="229" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B229" t="s">
         <v>264</v>
@@ -25465,7 +25465,7 @@
     </row>
     <row r="230" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B230" t="s">
         <v>264</v>
@@ -25531,7 +25531,7 @@
     </row>
     <row r="231" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B231" t="s">
         <v>264</v>
@@ -25597,7 +25597,7 @@
     </row>
     <row r="232" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B232" t="s">
         <v>264</v>
@@ -25663,7 +25663,7 @@
     </row>
     <row r="233" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B233" t="s">
         <v>264</v>
@@ -25729,7 +25729,7 @@
     </row>
     <row r="234" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B234" t="s">
         <v>264</v>
@@ -25795,7 +25795,7 @@
     </row>
     <row r="235" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B235" t="s">
         <v>264</v>
@@ -25861,7 +25861,7 @@
     </row>
     <row r="236" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B236" t="s">
         <v>264</v>
@@ -25927,7 +25927,7 @@
     </row>
     <row r="237" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B237" t="s">
         <v>264</v>
@@ -25993,7 +25993,7 @@
     </row>
     <row r="238" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B238" t="s">
         <v>264</v>
@@ -26059,7 +26059,7 @@
     </row>
     <row r="239" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B239" t="s">
         <v>264</v>
@@ -26125,7 +26125,7 @@
     </row>
     <row r="240" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B240" t="s">
         <v>264</v>
@@ -26191,7 +26191,7 @@
     </row>
     <row r="241" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B241" t="s">
         <v>264</v>
@@ -26257,7 +26257,7 @@
     </row>
     <row r="242" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B242" t="s">
         <v>264</v>
@@ -26323,7 +26323,7 @@
     </row>
     <row r="243" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B243" t="s">
         <v>264</v>
@@ -26389,7 +26389,7 @@
     </row>
     <row r="244" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B244" t="s">
         <v>45</v>
@@ -26455,7 +26455,7 @@
     </row>
     <row r="245" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B245" t="s">
         <v>45</v>
@@ -26521,7 +26521,7 @@
     </row>
     <row r="246" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B246" t="s">
         <v>45</v>
@@ -26587,7 +26587,7 @@
     </row>
     <row r="247" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B247" t="s">
         <v>45</v>
@@ -26653,7 +26653,7 @@
     </row>
     <row r="248" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B248" t="s">
         <v>45</v>
@@ -26719,7 +26719,7 @@
     </row>
     <row r="249" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B249" t="s">
         <v>45</v>
@@ -26785,7 +26785,7 @@
     </row>
     <row r="250" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B250" t="s">
         <v>45</v>
@@ -26851,7 +26851,7 @@
     </row>
     <row r="251" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B251" t="s">
         <v>45</v>
@@ -37634,7 +37634,7 @@
     </row>
     <row r="413" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B413" t="s">
         <v>612</v>
@@ -39072,7 +39072,7 @@
         <v>235</v>
       </c>
       <c r="T434" s="19" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="U434" s="19" t="s">
         <v>558</v>
@@ -41942,7 +41942,7 @@
         <v>764</v>
       </c>
       <c r="D478" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E478" s="3">
         <v>44711</v>
@@ -42140,7 +42140,7 @@
         <v>773</v>
       </c>
       <c r="D481" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E481" s="3">
         <v>44711</v>
@@ -42206,7 +42206,7 @@
         <v>774</v>
       </c>
       <c r="D482" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E482" s="3">
         <v>44711</v>
@@ -42272,7 +42272,7 @@
         <v>779</v>
       </c>
       <c r="D483" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E483" s="3">
         <v>44711</v>
@@ -42338,7 +42338,7 @@
         <v>772</v>
       </c>
       <c r="D484" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E484" s="3">
         <v>44711</v>
@@ -42407,7 +42407,7 @@
         <v>775</v>
       </c>
       <c r="D485" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E485" s="3">
         <v>44711</v>
@@ -42473,7 +42473,7 @@
         <v>776</v>
       </c>
       <c r="D486" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E486" s="3">
         <v>44711</v>
@@ -42539,7 +42539,7 @@
         <v>778</v>
       </c>
       <c r="D487" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E487" s="3">
         <v>44711</v>
@@ -42605,7 +42605,7 @@
         <v>777</v>
       </c>
       <c r="D488" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E488" s="3">
         <v>44711</v>
@@ -42668,13 +42668,13 @@
         <v>763</v>
       </c>
       <c r="B489" s="12" t="s">
+        <v>825</v>
+      </c>
+      <c r="C489" t="s">
         <v>780</v>
       </c>
-      <c r="C489" t="s">
-        <v>781</v>
-      </c>
       <c r="D489" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E489" s="3">
         <v>44711</v>
@@ -42731,13 +42731,13 @@
         <v>763</v>
       </c>
       <c r="B490" s="17" t="s">
-        <v>780</v>
+        <v>825</v>
       </c>
       <c r="C490" s="4" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D490" s="4" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E490" s="18">
         <v>44711</v>
@@ -42786,7 +42786,7 @@
         <v>233</v>
       </c>
       <c r="T490" s="4" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="U490" t="s">
         <v>301</v>
@@ -42800,13 +42800,13 @@
         <v>763</v>
       </c>
       <c r="B491" s="17" t="s">
-        <v>780</v>
+        <v>825</v>
       </c>
       <c r="C491" s="4" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D491" s="4" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E491" s="18">
         <v>44711</v>
@@ -42855,7 +42855,7 @@
         <v>233</v>
       </c>
       <c r="T491" s="4" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="U491" t="s">
         <v>301</v>
@@ -42869,13 +42869,13 @@
         <v>763</v>
       </c>
       <c r="B492" s="12" t="s">
-        <v>780</v>
+        <v>825</v>
       </c>
       <c r="C492" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D492" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E492" s="3">
         <v>44711</v>
@@ -42935,13 +42935,13 @@
         <v>763</v>
       </c>
       <c r="B493" s="12" t="s">
-        <v>780</v>
+        <v>825</v>
       </c>
       <c r="C493" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D493" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E493" s="3">
         <v>44711</v>
@@ -43001,13 +43001,13 @@
         <v>763</v>
       </c>
       <c r="B494" s="12" t="s">
-        <v>780</v>
+        <v>825</v>
       </c>
       <c r="C494" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D494" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E494" s="3">
         <v>44711</v>
@@ -43067,13 +43067,13 @@
         <v>763</v>
       </c>
       <c r="B495" s="12" t="s">
-        <v>780</v>
+        <v>825</v>
       </c>
       <c r="C495" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D495" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E495" s="3">
         <v>44711</v>
@@ -43133,13 +43133,13 @@
         <v>763</v>
       </c>
       <c r="B496" s="12" t="s">
-        <v>780</v>
+        <v>825</v>
       </c>
       <c r="C496" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D496" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E496" s="3">
         <v>44711</v>
@@ -43199,13 +43199,13 @@
         <v>763</v>
       </c>
       <c r="B497" s="12" t="s">
-        <v>780</v>
+        <v>825</v>
       </c>
       <c r="C497" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="D497" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E497" s="3">
         <v>44711</v>
@@ -43265,13 +43265,13 @@
         <v>763</v>
       </c>
       <c r="B498" s="12" t="s">
-        <v>780</v>
+        <v>825</v>
       </c>
       <c r="C498" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D498" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E498" s="3">
         <v>44711</v>
@@ -43331,13 +43331,13 @@
         <v>763</v>
       </c>
       <c r="B499" s="12" t="s">
-        <v>780</v>
+        <v>825</v>
       </c>
       <c r="C499" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D499" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E499" s="3">
         <v>44711</v>
@@ -43397,13 +43397,13 @@
         <v>763</v>
       </c>
       <c r="B500" s="12" t="s">
-        <v>780</v>
+        <v>825</v>
       </c>
       <c r="C500" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D500" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E500" s="3">
         <v>44711</v>
@@ -43463,13 +43463,13 @@
         <v>690</v>
       </c>
       <c r="B501" s="22" t="s">
+        <v>793</v>
+      </c>
+      <c r="C501" s="19" t="s">
+        <v>801</v>
+      </c>
+      <c r="D501" s="19" t="s">
         <v>794</v>
-      </c>
-      <c r="C501" s="19" t="s">
-        <v>802</v>
-      </c>
-      <c r="D501" s="19" t="s">
-        <v>795</v>
       </c>
       <c r="E501" s="20">
         <v>44711</v>
@@ -43518,7 +43518,7 @@
         <v>233</v>
       </c>
       <c r="T501" s="19" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="U501" s="19" t="s">
         <v>558</v>
@@ -43532,13 +43532,13 @@
         <v>690</v>
       </c>
       <c r="B502" s="12" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C502" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D502" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E502" s="3">
         <v>44711</v>
@@ -43598,13 +43598,13 @@
         <v>690</v>
       </c>
       <c r="B503" s="12" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C503" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D503" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E503" s="3">
         <v>44711</v>
@@ -43664,13 +43664,13 @@
         <v>690</v>
       </c>
       <c r="B504" s="12" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C504" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D504" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E504" s="3">
         <v>44711</v>
@@ -43730,13 +43730,13 @@
         <v>690</v>
       </c>
       <c r="B505" s="22" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C505" s="19" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D505" s="19" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E505" s="20">
         <v>44711</v>
@@ -43785,7 +43785,7 @@
         <v>233</v>
       </c>
       <c r="T505" s="19" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="U505" s="19" t="s">
         <v>558</v>
@@ -43799,13 +43799,13 @@
         <v>690</v>
       </c>
       <c r="B506" s="22" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C506" s="19" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D506" s="19" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E506" s="20">
         <v>44711</v>
@@ -43854,7 +43854,7 @@
         <v>233</v>
       </c>
       <c r="T506" s="19" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="U506" s="19" t="s">
         <v>558</v>
@@ -43868,13 +43868,13 @@
         <v>690</v>
       </c>
       <c r="B507" s="22" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C507" s="19" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D507" s="19" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E507" s="20">
         <v>44711</v>
@@ -43923,7 +43923,7 @@
         <v>233</v>
       </c>
       <c r="T507" s="19" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="U507" s="19" t="s">
         <v>558</v>
@@ -43940,10 +43940,10 @@
         <v>581</v>
       </c>
       <c r="C508" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D508" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E508" s="3">
         <v>44711</v>
@@ -44006,10 +44006,10 @@
         <v>581</v>
       </c>
       <c r="C509" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D509" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E509" s="3">
         <v>44711</v>
@@ -44072,10 +44072,10 @@
         <v>581</v>
       </c>
       <c r="C510" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D510" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E510" s="3">
         <v>44711</v>
@@ -44138,10 +44138,10 @@
         <v>581</v>
       </c>
       <c r="C511" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D511" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E511" s="3">
         <v>44711</v>
@@ -44214,7 +44214,7 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
@@ -44380,7 +44380,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.26953125" bestFit="1" customWidth="1"/>
@@ -44463,7 +44463,7 @@
         <v>773</v>
       </c>
       <c r="B10" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -44471,7 +44471,7 @@
         <v>774</v>
       </c>
       <c r="B11" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -44479,7 +44479,7 @@
         <v>779</v>
       </c>
       <c r="B12" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -44487,7 +44487,7 @@
         <v>775</v>
       </c>
       <c r="B13" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -44495,7 +44495,7 @@
         <v>776</v>
       </c>
       <c r="B14" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -44503,63 +44503,63 @@
         <v>778</v>
       </c>
       <c r="B15" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B16" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B17" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B18" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B19" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B20" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B21" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B22" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
   </sheetData>

</xml_diff>